<commit_message>
backend tranfered to express
</commit_message>
<xml_diff>
--- a/backend/ScrapBackend/scrapping/Excels/Quess_AmbitionBox-overalldata.xlsx
+++ b/backend/ScrapBackend/scrapping/Excels/Quess_AmbitionBox-overalldata.xlsx
@@ -441,7 +441,7 @@
         <v>1.3k</v>
       </c>
       <c r="E2" t="str">
-        <v>718</v>
+        <v>722</v>
       </c>
       <c r="F2" t="str">
         <v>264</v>
@@ -492,233 +492,233 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Java J2ee Developer</v>
+        <v>Jdss</v>
       </c>
       <c r="B2" t="str">
-        <v>Noida</v>
+        <v>Bangalore / Bengaluru</v>
       </c>
       <c r="D2" t="str">
         <v>Full Time</v>
       </c>
       <c r="E2" t="str">
-        <v>30 Apr 2024</v>
+        <v>02 May 2024</v>
       </c>
       <c r="F2" t="str">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="G2" t="str">
-        <v>if you are a fresher and you dont have other offers then join otherwise DON'T</v>
+        <v>No such thing to like , because company was worst</v>
       </c>
       <c r="H2" t="str">
-        <v>No communication from manager or HR. They will just deploy you to client location and never contact you ever again.</v>
+        <v>Without any notice they will fired, hr was not good, not giving fixed salary</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Senior Sales Executive</v>
+        <v>Java J2ee Developer</v>
       </c>
       <c r="B3" t="str">
-        <v>Coimbatore</v>
+        <v>Noida</v>
       </c>
       <c r="D3" t="str">
-        <v>Software Development Department</v>
+        <v>Sales Support &amp; Operations Department</v>
       </c>
       <c r="E3" t="str">
         <v>30 Apr 2024</v>
       </c>
       <c r="F3" t="str">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="G3" t="str">
-        <v>Nothing</v>
+        <v>if you are a fresher and you dont have other offers then join otherwise DON'T</v>
       </c>
       <c r="H3" t="str">
-        <v>I have worked there past 8.3years. But i didn't not received relieving letter. You are spoiled my carrier. I already told about the visiting card issue to my manager, they also know about the issue. But I'm a off role employee. Company never consider my career. Totally i disappointed to work witthis company.</v>
+        <v>No communication from manager or HR. They will just deploy you to client location and never contact you ever again.</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Senior Business Analyst</v>
+        <v>Senior Sales Executive</v>
       </c>
       <c r="B4" t="str">
-        <v>Bangalore / Bengaluru</v>
+        <v>Coimbatore</v>
       </c>
       <c r="D4" t="str">
         <v>Full Time</v>
       </c>
       <c r="E4" t="str">
-        <v>28 Apr 2024</v>
+        <v>30 Apr 2024</v>
       </c>
       <c r="F4" t="str">
         <v>1.0</v>
       </c>
       <c r="G4" t="str">
-        <v>Quess is such a pathetic company to work.They end their staff's contract without proper notice and show so much of unprofessional behaviour.</v>
+        <v>Nothing</v>
       </c>
       <c r="H4" t="str">
-        <v>Job security</v>
-      </c>
-    </row>
-    <row r="5" xml:space="preserve">
+        <v>I have worked there past 8.3years. But i didn't not received relieving letter. You are spoiled my carrier. I already told about the visiting card issue to my manager, they also know about the issue. But I'm a off role employee. Company never consider my career. Totally i disappointed to work witthis company.</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="str">
-        <v>Marketing Manager</v>
+        <v>Senior Business Analyst</v>
       </c>
       <c r="B5" t="str">
-        <v>New Delhi</v>
+        <v>Bangalore / Bengaluru</v>
       </c>
       <c r="D5" t="str">
-        <v>Sales Support &amp; Operations Department</v>
+        <v>Software Development Department</v>
       </c>
       <c r="E5" t="str">
-        <v>23 Apr 2024</v>
+        <v>28 Apr 2024</v>
       </c>
       <c r="F5" t="str">
         <v>1.0</v>
       </c>
-      <c r="G5" t="str" xml:space="preserve">
+      <c r="G5" t="str">
+        <v>Quess is such a pathetic company to work.They end their staff's contract without proper notice and show so much of unprofessional behaviour.</v>
+      </c>
+      <c r="H5" t="str">
+        <v>Job security</v>
+      </c>
+    </row>
+    <row r="6" xml:space="preserve">
+      <c r="A6" t="str">
+        <v>Marketing Manager</v>
+      </c>
+      <c r="B6" t="str">
+        <v>New Delhi</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Full Time</v>
+      </c>
+      <c r="E6" t="str">
+        <v>23 Apr 2024</v>
+      </c>
+      <c r="F6" t="str">
+        <v>1.0</v>
+      </c>
+      <c r="G6" t="str" xml:space="preserve">
         <v xml:space="preserve">Poor culture they are not allow to take leave even an emergency condition.
 they are not willing to get promoted .</v>
       </c>
-      <c r="H5" t="str">
+      <c r="H6" t="str">
         <v>culture, rude behavior, poor enviornment</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Vocational Trainer</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Hosapete</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Full Time</v>
-      </c>
-      <c r="E6" t="str">
-        <v>17 Mar 2024</v>
-      </c>
-      <c r="F6" t="str">
-        <v>5.0</v>
-      </c>
-      <c r="G6" t="str">
-        <v>Since I have joined as a vocational trainer on 2022 I have a very good experience and I'm happy also about my work too am.As quess is providing employment for us without any experience it s a good matter</v>
-      </c>
-      <c r="H6" t="str">
-        <v>Salary is quite is less and no increments</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Vice President Operations</v>
+        <v>Vocational Trainer</v>
       </c>
       <c r="B7" t="str">
-        <v>Bangalore / Bengaluru</v>
+        <v>Hosapete</v>
       </c>
       <c r="D7" t="str">
-        <v>IT Infrastructure Services Department</v>
+        <v>Sales Support &amp; Operations Department</v>
       </c>
       <c r="E7" t="str">
-        <v>05 Mar 2024</v>
+        <v>17 Mar 2024</v>
       </c>
       <c r="F7" t="str">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="G7" t="str">
-        <v>It's an Indian company with a multinational culture. Gives the flexibility to work for an individual with very less</v>
+        <v>Since I have joined as a vocational trainer on 2022 I have a very good experience and I'm happy also about my work too am.As quess is providing employment for us without any experience it s a good matter</v>
       </c>
       <c r="H7" t="str">
-        <v>Management believes few of the initial people except that they don't believe the key people as well.</v>
+        <v>Salary is quite is less and no increments</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Senior Stylist</v>
+        <v>Vice President Operations</v>
       </c>
       <c r="B8" t="str">
-        <v>Hyderabad / Secunderabad</v>
+        <v>Bangalore / Bengaluru</v>
       </c>
       <c r="D8" t="str">
         <v>Full Time</v>
       </c>
       <c r="E8" t="str">
-        <v>26 Feb 2024</v>
+        <v>05 Mar 2024</v>
       </c>
       <c r="F8" t="str">
         <v>4.0</v>
       </c>
       <c r="G8" t="str">
-        <v>The first thing I like is we got salaries on time and that to on 1st day of the month</v>
+        <v>It's an Indian company with a multinational culture. Gives the flexibility to work for an individual with very less</v>
       </c>
       <c r="H8" t="str">
-        <v>It should be more good when compared to other companies.</v>
+        <v>Management believes few of the initial people except that they don't believe the key people as well.</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Senior Accounts Executive</v>
+        <v>Senior Stylist</v>
       </c>
       <c r="B9" t="str">
-        <v>Bangalore / Bengaluru (working remotely)</v>
+        <v>Hyderabad / Secunderabad</v>
       </c>
       <c r="D9" t="str">
-        <v>Marketing Department</v>
+        <v>IT Infrastructure Services Department</v>
       </c>
       <c r="E9" t="str">
-        <v>20 Feb 2024</v>
+        <v>26 Feb 2024</v>
       </c>
       <c r="F9" t="str">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="G9" t="str">
-        <v>there is nothing to say about it</v>
+        <v>The first thing I like is we got salaries on time and that to on 1st day of the month</v>
       </c>
       <c r="H9" t="str">
-        <v>worst management, no recognition given to the employees, huge work pressure on single employee, kindly don't join here</v>
+        <v>It should be more good when compared to other companies.</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Data Center Engineer</v>
+        <v>Senior Accounts Executive</v>
       </c>
       <c r="B10" t="str">
-        <v>Hyderabad / Secunderabad</v>
+        <v>Bangalore / Bengaluru (working remotely)</v>
       </c>
       <c r="D10" t="str">
         <v>Full Time</v>
       </c>
       <c r="E10" t="str">
-        <v>10 Feb 2024</v>
+        <v>20 Feb 2024</v>
       </c>
       <c r="F10" t="str">
         <v>1.0</v>
       </c>
       <c r="G10" t="str">
-        <v>Didn't know till</v>
+        <v>there is nothing to say about it</v>
       </c>
       <c r="H10" t="str">
-        <v>Company for clients only, didn't care for employees and they do whatever client asks and forcing employees to do that</v>
+        <v>worst management, no recognition given to the employees, huge work pressure on single employee, kindly don't join here</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Field Engineer</v>
+        <v>Data Center Engineer</v>
       </c>
       <c r="B11" t="str">
-        <v>Biswan</v>
+        <v>Hyderabad / Secunderabad</v>
       </c>
       <c r="D11" t="str">
-        <v>Engineering Department</v>
+        <v>Marketing Department</v>
       </c>
       <c r="E11" t="str">
-        <v>05 Feb 2024</v>
+        <v>10 Feb 2024</v>
       </c>
       <c r="F11" t="str">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="G11" t="str">
-        <v>Skilled IT Engineer with [1years] of experience in designing, implementing, and managing IT systems. Adept at troubleshooting complex technical issues and implementing effective solutions. Seeking to contribute technical expertise to a dynamic IT team.</v>
+        <v>Didn't know till</v>
       </c>
       <c r="H11" t="str">
-        <v>All best but tender only 1 year's</v>
+        <v>Company for clients only, didn't care for employees and they do whatever client asks and forcing employees to do that</v>
       </c>
     </row>
   </sheetData>

</xml_diff>